<commit_message>
trying to fix issue with pictures now showing up in nbviewer.jupyter.org
</commit_message>
<xml_diff>
--- a/logit_curve_only.xlsx
+++ b/logit_curve_only.xlsx
@@ -41,8 +41,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt formatCode="yyyy-mm-dd h:mm:ss" numFmtId="164"/>
+    <numFmt formatCode="YYYY-MM-DD HH:MM:SS" numFmtId="165"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -88,7 +89,7 @@
     <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>

</xml_diff>